<commit_message>
improving upload excel for laporanTp, adding E7 and L2 to PEARLS, and refactoring laporanCuController query
</commit_message>
<xml_diff>
--- a/public/files/formatLaporanCu.xlsx
+++ b/public/files/formatLaporanCu.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Sites/bkcuvue/public/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\bkcuvue\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B2C1620-69CE-DA47-8A63-D9283FEF67D4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDEA1DA-8F35-4DC7-B129-271A1A09B104}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="27320" windowHeight="14900" xr2:uid="{6E3E5F2B-8BA1-F845-BBF4-F30D4ACC6EF2}"/>
+    <workbookView xWindow="28800" yWindow="465" windowWidth="27315" windowHeight="14895" xr2:uid="{6E3E5F2B-8BA1-F845-BBF4-F30D4ACC6EF2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>lelaki biasa</t>
   </si>
@@ -135,10 +135,13 @@
     <t>harga pasar</t>
   </si>
   <si>
-    <t>tgl buat</t>
-  </si>
-  <si>
     <t>periode</t>
+  </si>
+  <si>
+    <t>aset_likuid_tidak_menghasilkan</t>
+  </si>
+  <si>
+    <t>tanggal buat</t>
   </si>
 </sst>
 </file>
@@ -490,166 +493,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B728F6F-ED4D-754B-AFD8-5624DAAEA7F5}">
-  <dimension ref="A1:AL1"/>
+  <dimension ref="A1:AM1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>36</v>
+      <c r="AM1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>